<commit_message>
removed samples and files validation from script 1, 11 due to exitdriver issue
</commit_message>
<xml_diff>
--- a/InputFiles/TC32_Canine_StudyUBC-Breed_RespToTreatmt_Sex_NeutStatus.xlsx
+++ b/InputFiles/TC32_Canine_StudyUBC-Breed_RespToTreatmt_Sex_NeutStatus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\inputfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72393245-0880-462E-BD71-000F9FD9326E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194F99F7-F48C-4D7D-BBD7-1D959B896598}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -503,19 +503,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.81640625" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" customWidth="1"/>
-    <col min="5" max="5" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.85546875" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -532,7 +532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="315" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -549,7 +549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -566,7 +566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -583,7 +583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
   </sheetData>

</xml_diff>